<commit_message>
Fixed comment field for Diodes TVS (Bi-directional) and Mounting hole
</commit_message>
<xml_diff>
--- a/BOM/Template_BOM.xlsx
+++ b/BOM/Template_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EL-sense\Altium_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EL-sense\Altium_Library\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5F53013-99C1-4C4E-AFEB-6380B1E01ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C3A057-25BA-4E0F-B161-E5D7F22B961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -130,15 +130,9 @@
     <t>Print Date:</t>
   </si>
   <si>
-    <t>Column=Description</t>
-  </si>
-  <si>
     <t>Report Date:</t>
   </si>
   <si>
-    <t>Component list</t>
-  </si>
-  <si>
     <t>Column=Quantity</t>
   </si>
   <si>
@@ -148,24 +142,15 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Column=Category</t>
   </si>
   <si>
-    <t>Column=Supplier Part Number 1</t>
-  </si>
-  <si>
     <t>Column=Supplier Order Qty 1</t>
   </si>
   <si>
     <t>Column=Supplier Stock 1</t>
   </si>
   <si>
-    <t>Column=Supplier Unit Price 1</t>
-  </si>
-  <si>
     <t>Column=Supplier Subtotal 1</t>
   </si>
   <si>
@@ -218,6 +203,24 @@
   </si>
   <si>
     <t>Column=Supplier</t>
+  </si>
+  <si>
+    <t>Column=Item</t>
+  </si>
+  <si>
+    <t>Column=Designator</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Bill of Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column=Description  </t>
+  </si>
+  <si>
+    <t>Supplier Unit Price</t>
   </si>
 </sst>
 </file>
@@ -228,16 +231,10 @@
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <u/>
@@ -246,71 +243,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -327,48 +259,127 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
+      <sz val="24"/>
       <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="7">
@@ -815,10 +826,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -827,61 +838,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -923,333 +880,397 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1349,14 +1370,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>128307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -1386,7 +1407,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13201650" y="776007"/>
+          <a:off x="18992850" y="776007"/>
           <a:ext cx="1200150" cy="1043268"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1723,463 +1744,483 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="96" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="86" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="86" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="86" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" style="85" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="11" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="76"/>
-    </row>
-    <row r="2" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="30"/>
+    <row r="1" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="90"/>
+    </row>
+    <row r="2" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="85"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
-      <c r="O2" s="77"/>
-    </row>
-    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="68"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="19" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="48"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="78"/>
-    </row>
-    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="78"/>
-    </row>
-    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="74" t="s">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="23"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="89">
+        <f ca="1">TODAY()</f>
+        <v>44635</v>
+      </c>
+      <c r="E8" s="107">
+        <f ca="1">NOW()</f>
+        <v>44635.770101504633</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="23"/>
+    </row>
+    <row r="9" spans="1:16" s="42" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="78"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="68"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="78"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="68"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+      <c r="F9" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="78"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="68"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="27">
-        <f ca="1">TODAY()</f>
-        <v>44610</v>
-      </c>
-      <c r="E8" s="28">
-        <f ca="1">NOW()</f>
-        <v>44610.898766782404</v>
-      </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="78"/>
-    </row>
-    <row r="9" spans="1:15" s="47" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
-      <c r="B9" s="44" t="s">
+      <c r="K9" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="N9" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="45" t="s">
+      <c r="P9" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" s="46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68"/>
-      <c r="B10" s="37">
+    </row>
+    <row r="10" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="43">
         <f>ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="79"/>
-    </row>
-    <row r="11" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="68"/>
-      <c r="B11" s="39">
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="92"/>
+    </row>
+    <row r="11" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="47">
         <f>ROW(B11) - ROW($B$9)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="80"/>
-    </row>
-    <row r="12" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68"/>
-      <c r="B12" s="40">
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="93"/>
+    </row>
+    <row r="12" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="51">
         <f>ROW(B12) - ROW($B$9)</f>
         <v>3</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="52"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="105"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="81"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="68"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="59">
-        <f>SUM(H10:H12)</f>
+      <c r="M12" s="53"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="94"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="60">
+        <f>SUM(J10:J12)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="92"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="59">
-        <f>SUM(K10:K12)</f>
+      <c r="K13" s="61"/>
+      <c r="L13" s="60">
+        <f>SUM(L10:L12)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58">
-        <f>SUM(N10:N12)</f>
+      <c r="M13" s="60"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62">
+        <f>SUM(O10:O12)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="82"/>
-    </row>
-    <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
-      <c r="B14" s="103" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="103"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="78"/>
-    </row>
-    <row r="15" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="68"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="98" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="48"/>
-      <c r="L15" s="104">
-        <f>N13</f>
+      <c r="P13" s="63"/>
+    </row>
+    <row r="14" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="95"/>
+    </row>
+    <row r="15" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="20"/>
+      <c r="N15" s="75">
+        <f>P13</f>
         <v>0</v>
       </c>
-      <c r="M15" s="105"/>
-      <c r="N15" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="O15" s="78"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="68"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="106" t="e">
-        <f>L15/H15</f>
+      <c r="O15" s="87"/>
+      <c r="P15" s="96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="70"/>
+      <c r="N16" s="77" t="e">
+        <f>N15/J15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M16" s="106"/>
-      <c r="N16" s="99" t="s">
-        <v>47</v>
-      </c>
-      <c r="O16" s="78"/>
-    </row>
-    <row r="17" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="83"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="78"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="97"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="L10:L12">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="M10:M12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10:N12">
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(N10))=0</formula>
+  <conditionalFormatting sqref="O10:O12">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(O10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -2208,114 +2249,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[update] New version of technical information, symbols and footprints for resistors
</commit_message>
<xml_diff>
--- a/BOM/Template_BOM.xlsx
+++ b/BOM/Template_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EL-sense\Altium_Library\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705FAA9-B4C0-49A6-98AC-135C1BF1707D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BFE063-5410-46BD-BCB9-3FA21FCD3473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -187,15 +187,9 @@
     <t>Column=Manufacturer</t>
   </si>
   <si>
-    <t>Column=Part Number</t>
-  </si>
-  <si>
     <t>Column=Case</t>
   </si>
   <si>
-    <t>Column=Supplier</t>
-  </si>
-  <si>
     <t>Column=Item</t>
   </si>
   <si>
@@ -211,13 +205,19 @@
     <t xml:space="preserve">Column=Description  </t>
   </si>
   <si>
-    <t>Supplier Unit Price</t>
-  </si>
-  <si>
     <t>Revision:</t>
   </si>
   <si>
     <t>Field=ProjectRevision</t>
+  </si>
+  <si>
+    <t>Column=Supplier 1</t>
+  </si>
+  <si>
+    <t>Column=Supplier Part Number 1</t>
+  </si>
+  <si>
+    <t>Column=Supplier Unit Price 1</t>
   </si>
 </sst>
 </file>
@@ -384,18 +384,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -434,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -703,32 +697,6 @@
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -937,24 +905,24 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -963,47 +931,47 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1024,7 +992,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1033,7 +1001,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1108,153 +1076,136 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="21" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1731,7 +1682,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1777,7 +1728,7 @@
       <c r="A2" s="70"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
@@ -1873,10 +1824,10 @@
       <c r="A6" s="70"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="24"/>
@@ -1921,13 +1872,13 @@
       <c r="C8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="101">
+      <c r="D8" s="89">
         <f ca="1">TODAY()</f>
-        <v>44743</v>
-      </c>
-      <c r="E8" s="102">
+        <v>44767</v>
+      </c>
+      <c r="E8" s="90">
         <f ca="1">NOW()</f>
-        <v>44743.89474895833</v>
+        <v>44767.722890509256</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="25"/>
@@ -1943,49 +1894,49 @@
     </row>
     <row r="9" spans="1:16" s="28" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="92" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="92" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="92" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="92" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="104" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="104" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="104" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="104" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="104" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="104" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="105" t="s">
+      <c r="M9" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="105" t="s">
-        <v>59</v>
-      </c>
-      <c r="O9" s="105" t="s">
+      <c r="N9" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="106" t="s">
+      <c r="P9" s="94" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2005,52 +1956,52 @@
       <c r="J10" s="77"/>
       <c r="K10" s="76"/>
       <c r="L10" s="77"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="81"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="79"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="70"/>
-      <c r="B11" s="96">
+      <c r="B11" s="85">
         <f>ROW(B11) - ROW($B$9)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="97"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97"/>
-      <c r="H11" s="97"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="100"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="88"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="70"/>
-      <c r="B12" s="84">
+      <c r="B12" s="80">
         <f>ROW(B12) - ROW($B$9)</f>
         <v>3</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="91"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="84"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="70"/>
@@ -2081,10 +2032,10 @@
     </row>
     <row r="14" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="70"/>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="92"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="38"/>
       <c r="E14" s="39"/>
       <c r="F14" s="40" t="s">
@@ -2121,11 +2072,11 @@
         <v>41</v>
       </c>
       <c r="M15" s="12"/>
-      <c r="N15" s="93">
+      <c r="N15" s="96">
         <f>O13</f>
         <v>0</v>
       </c>
-      <c r="O15" s="94"/>
+      <c r="O15" s="97"/>
       <c r="P15" s="59" t="s">
         <v>42</v>
       </c>
@@ -2146,11 +2097,11 @@
         <v>47</v>
       </c>
       <c r="M16" s="43"/>
-      <c r="N16" s="95" t="e">
+      <c r="N16" s="98" t="e">
         <f>N15/J15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O16" s="95"/>
+      <c r="O16" s="98"/>
       <c r="P16" s="15" t="s">
         <v>42</v>
       </c>
@@ -2195,16 +2146,6 @@
     <mergeCell ref="N16:O16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="M10:M12">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O10:O12">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(O10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">

</xml_diff>